<commit_message>
Filling up the clean new PDF
</commit_message>
<xml_diff>
--- a/dataBase/items.xlsx
+++ b/dataBase/items.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607B15A8-CFAE-40A6-9BD1-A93F605BE9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Armors" sheetId="1" r:id="rId1"/>
+    <sheet name="Shields" sheetId="3" r:id="rId2"/>
+    <sheet name="Weapons" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,15 +26,100 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>handle</t>
+  </si>
+  <si>
+    <t>specials</t>
+  </si>
+  <si>
+    <t>Pałka</t>
+  </si>
+  <si>
+    <t>1k6</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Kostur</t>
+  </si>
+  <si>
+    <t>Proca</t>
+  </si>
+  <si>
+    <t>1k6+1</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>Finezyjna</t>
+  </si>
+  <si>
+    <t>1k3</t>
+  </si>
+  <si>
+    <t>1H/2H</t>
+  </si>
+  <si>
+    <t>Używa kamieni, zasięg (średni)</t>
+  </si>
+  <si>
+    <t>Sztylet</t>
+  </si>
+  <si>
+    <t>Finezyjna, miotana, zasięg (bliski)</t>
+  </si>
+  <si>
+    <t>Mała Tarcza</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>Defensywna +1</t>
+  </si>
+  <si>
+    <t>Duża Tarcza</t>
+  </si>
+  <si>
+    <t>Defensuwa +2, Rozmiar 1</t>
+  </si>
+  <si>
+    <t>Miecz</t>
+  </si>
+  <si>
+    <t>1k6+2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Metropolis-Regular"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,11 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +424,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F4D615-B536-42D1-BDC3-CE727F913D46}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B78F2F5-7D3E-479E-86EE-4145D68F45B7}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed addding statistics of weapons  and fixed in database profesions
</commit_message>
<xml_diff>
--- a/dataBase/items.xlsx
+++ b/dataBase/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607B15A8-CFAE-40A6-9BD1-A93F605BE9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07232B29-9D46-48E9-A28C-BAB3C66E9A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="8565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>1H</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Kostur</t>
   </si>
   <si>
@@ -102,6 +99,15 @@
   </si>
   <si>
     <t>1k6+2</t>
+  </si>
+  <si>
+    <t>brak</t>
+  </si>
+  <si>
+    <t>Pancerz</t>
+  </si>
+  <si>
+    <t>features</t>
   </si>
 </sst>
 </file>
@@ -427,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -442,21 +448,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -491,10 +497,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -502,13 +508,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -520,11 +526,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B78F2F5-7D3E-479E-86EE-4145D68F45B7}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -551,7 +560,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -559,55 +568,55 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>